<commit_message>
Updated codeboks and "added" logo
</commit_message>
<xml_diff>
--- a/i_codebooks/D5_Table_3_Covariates_ImmDis.xlsx
+++ b/i_codebooks/D5_Table_3_Covariates_ImmDis.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20415"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\ROC18_Objective_2\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\ROC18_Objective_2\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D337150-2D70-46CB-B728-2F399127E3FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="462">
   <si>
     <t>metadata_content</t>
   </si>
@@ -1422,11 +1423,14 @@
   <si>
     <t>D5_Table_3_Covariates_{ImmDis}</t>
   </si>
+  <si>
+    <t>empty</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -1730,7 +1734,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2007,16 +2011,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2028,7 +2032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="28.8">
+    <row r="2" spans="1:2" ht="30">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
@@ -2102,7 +2106,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2112,20 +2116,20 @@
       <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="11"/>
-    <col min="2" max="2" width="56.33203125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" style="11" customWidth="1"/>
-    <col min="7" max="7" width="31.21875" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="11"/>
+    <col min="2" max="2" width="56.28515625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.77734375" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.77734375" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="8.6640625" style="11"/>
+    <col min="9" max="9" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.7109375" style="11" customWidth="1"/>
+    <col min="12" max="16384" width="8.7109375" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2164,7 +2168,7 @@
       </c>
       <c r="L1" s="10"/>
     </row>
-    <row r="2" spans="1:12" ht="158.4">
+    <row r="2" spans="1:12" ht="180">
       <c r="A2" s="12" t="s">
         <v>38</v>
       </c>
@@ -2296,20 +2300,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
+    <sheetView topLeftCell="A280" workbookViewId="0">
       <selection activeCell="B269" sqref="B269"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.109375" customWidth="1"/>
-    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -6450,20 +6454,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="115.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.21875" customWidth="1"/>
+    <col min="1" max="1" width="115.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6">
+    <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="15"/>
       <c r="B1" s="16" t="s">
         <v>1</v>
@@ -6496,7 +6500,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.6">
+    <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="3" t="s">
         <v>55</v>
       </c>
@@ -6504,13 +6508,13 @@
         <v>456</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6">
+    <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="36" t="s">
         <v>458</v>
       </c>
       <c r="B3" s="7"/>
     </row>
-    <row r="4" spans="1:11" ht="15.6">
+    <row r="4" spans="1:11" ht="15.75">
       <c r="A4" s="7" t="s">
         <v>455</v>
       </c>
@@ -6518,11 +6522,11 @@
         <v>457</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.6">
+    <row r="5" spans="1:11" ht="15.75">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="15.6">
+    <row r="6" spans="1:11" ht="15.75">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
     </row>
@@ -6533,17 +6537,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="82.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="82.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>